<commit_message>
Fixed Lifting gear manager import issue
</commit_message>
<xml_diff>
--- a/files/system/import-shackles-sample.xlsx
+++ b/files/system/import-shackles-sample.xlsx
@@ -471,9 +471,7 @@
   <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="0" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W3" activeCellId="0" sqref="W3"/>
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>